<commit_message>
Update NewSmena and CreateElem
</commit_message>
<xml_diff>
--- a/fick1.xlsx
+++ b/fick1.xlsx
@@ -42,13 +42,13 @@
     <t>`</t>
   </si>
   <si>
+    <t>Корякин Н.Ю</t>
+  </si>
+  <si>
+    <t>xuyyyyy</t>
+  </si>
+  <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>Корякин Н.Ю</t>
-  </si>
-  <si>
-    <t>xuyyyyy</t>
   </si>
   <si>
     <t xml:space="preserve">Бушков </t>
@@ -692,8 +692,8 @@
   </sheetPr>
   <dimension ref="A1:AL29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -870,22 +870,22 @@
       </c>
       <c r="AA2" s="5" t="n"/>
       <c r="AB2" s="5" t="n"/>
-      <c r="AC2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>8</v>
+      <c r="AC2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="5" t="n">
+        <v>1</v>
       </c>
       <c r="AE2" s="5" t="n"/>
       <c r="AF2" s="1" t="n"/>
       <c r="AG2" s="5" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="AH2" s="5" t="n">
         <v>800</v>
       </c>
       <c r="AI2" s="5" t="n">
-        <v>11200</v>
+        <v>13600</v>
       </c>
       <c r="AJ2" s="5" t="n"/>
       <c r="AK2" s="5" t="n"/>
@@ -895,10 +895,10 @@
     </row>
     <row customHeight="1" ht="30" r="3" spans="1:38">
       <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>1</v>
@@ -931,31 +931,31 @@
       <c r="Q3" s="5" t="n"/>
       <c r="R3" s="6" t="n"/>
       <c r="S3" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="U3" s="5" t="n"/>
       <c r="V3" s="5" t="n"/>
       <c r="W3" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Y3" s="5" t="n"/>
       <c r="Z3" s="5" t="n"/>
       <c r="AA3" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AC3" s="5" t="n"/>
       <c r="AD3" s="5" t="n"/>
       <c r="AE3" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AF3" s="1" t="n"/>
       <c r="AG3" s="5" t="n">
@@ -1157,7 +1157,7 @@
     </row>
     <row r="20" spans="1:38">
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:38">
@@ -1214,7 +1214,7 @@
         <v>43314</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>13</v>
@@ -1236,7 +1236,7 @@
         <v>43256</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>13</v>
@@ -1258,7 +1258,7 @@
         <v>43319</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>13</v>
@@ -1269,7 +1269,7 @@
         <v>43320</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>13</v>
@@ -1280,7 +1280,7 @@
         <v>43322</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>13</v>
@@ -1291,7 +1291,7 @@
         <v>43344</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>19</v>
@@ -1302,7 +1302,7 @@
         <v>43345</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>20</v>
@@ -1313,7 +1313,7 @@
         <v>43348</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>20</v>
@@ -1324,7 +1324,7 @@
         <v>43348</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>20</v>
@@ -1368,7 +1368,7 @@
         <v>43352</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>20</v>
@@ -1379,7 +1379,7 @@
         <v>43353</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>20</v>
@@ -1390,7 +1390,7 @@
         <v>43354</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>20</v>
@@ -1423,7 +1423,7 @@
         <v>43357</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>23</v>
@@ -1515,7 +1515,7 @@
         <v>43345</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>33</v>
@@ -1557,7 +1557,7 @@
         <v>43348</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>38</v>
@@ -1578,7 +1578,7 @@
         <v>43348</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>40</v>
@@ -1660,7 +1660,7 @@
         <v>43352</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>47</v>
@@ -1681,7 +1681,7 @@
         <v>43358</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>49</v>

</xml_diff>